<commit_message>
Made cosmetic and wording changes to the Titan Park example and modified the rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab1/Assignment1Rubric.xlsx
+++ b/Labs/Lab1/Assignment1Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91AFA12-88E8-6D4A-ADD8-42405BD5770A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B200E4B1-0BD5-EC4D-8E71-8DCCF9FC458B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13640" yWindow="600" windowWidth="12600" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>CS246 Assignment 1 Rubric</t>
   </si>
@@ -51,18 +51,12 @@
     <t>Purpose and Scope</t>
   </si>
   <si>
-    <t>Stakeholders</t>
-  </si>
-  <si>
     <t>Functional Requirements</t>
   </si>
   <si>
     <t>Non-functional Requirements</t>
   </si>
   <si>
-    <t>Assumptions and Dependencies</t>
-  </si>
-  <si>
     <t>Data Requirements</t>
   </si>
   <si>
@@ -81,18 +75,6 @@
     <t>Sub-total</t>
   </si>
   <si>
-    <t>Questions and answers…</t>
-  </si>
-  <si>
-    <t>Are relevant to requirements</t>
-  </si>
-  <si>
-    <t>Include sifficent detail</t>
-  </si>
-  <si>
-    <t>Cover sufficent scope</t>
-  </si>
-  <si>
     <t>Requirements Doc</t>
   </si>
   <si>
@@ -102,20 +84,44 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Cover sufficient scope</t>
-  </si>
-  <si>
     <t>Answers include sufficient detail</t>
   </si>
   <si>
     <t>Qs ask for requirement details</t>
+  </si>
+  <si>
+    <t>Stakeholders and roles</t>
+  </si>
+  <si>
+    <t>Constraints, Assumptions &amp; Dependencies</t>
+  </si>
+  <si>
+    <t>Questions ask for requirement details</t>
+  </si>
+  <si>
+    <t>Questions are relevat to requirements</t>
+  </si>
+  <si>
+    <t>Questions cover sufficient scope</t>
+  </si>
+  <si>
+    <t>Constraints, Assumps, Deps</t>
+  </si>
+  <si>
+    <t>Qs are relevat to requirements</t>
+  </si>
+  <si>
+    <t>Qs over sufficient scope</t>
+  </si>
+  <si>
+    <t>As include sufficient detail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,11 +209,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Liberation Serif"/>
     </font>
     <font>
       <b/>
@@ -329,23 +330,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -360,20 +349,17 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -709,201 +695,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>SUM(B4:B12)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="9"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4">
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6">
+    <row r="19" spans="1:2">
+      <c r="A19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2">
+        <f>SUM(B16:B19)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9">
+    <row r="21" spans="1:2">
+      <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4">
-        <f>SUM(C4:C12)</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="4">
-        <f>SUM(C17:C22)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="4">
-        <f>C13+C23</f>
+      <c r="B22" s="2">
+        <f>B13+B20</f>
         <v>100</v>
       </c>
     </row>
@@ -918,51 +876,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="34">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="9" t="s">
-        <v>20</v>
+      <c r="A2" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="10"/>
+      <c r="A3" s="6"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
-        <v>21</v>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -971,11 +929,11 @@
       <c r="C5">
         <v>8</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="12" t="s">
-        <v>5</v>
+      <c r="A6" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -983,11 +941,11 @@
       <c r="C6">
         <v>6</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="12" t="s">
-        <v>6</v>
+      <c r="A7" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -995,15 +953,15 @@
       <c r="C7">
         <v>30</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="4"/>
       <c r="F7">
         <f>C7/B7</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="12" t="s">
-        <v>7</v>
+      <c r="A8" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -1011,11 +969,11 @@
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="12" t="s">
-        <v>8</v>
+      <c r="A9" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -1023,11 +981,11 @@
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
+      <c r="A10" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1035,11 +993,11 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
-        <v>10</v>
+      <c r="A11" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1047,11 +1005,11 @@
       <c r="C11">
         <v>3</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="12" t="s">
-        <v>11</v>
+      <c r="A12" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1059,11 +1017,11 @@
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="12" t="s">
-        <v>12</v>
+      <c r="A13" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1071,109 +1029,121 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
         <f>SUM(B5:B13)</f>
         <v>70</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <f>SUM(C5:C13)</f>
         <v>70</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
       <c r="F14">
         <f>C14/B14</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="13"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="9"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="8"/>
+      <c r="A16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="E17" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="12" t="s">
-        <v>22</v>
+      <c r="A18" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>10</v>
-      </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" s="18" customFormat="1">
-      <c r="A19" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="16">
-        <v>10</v>
-      </c>
-      <c r="C19" s="16">
-        <v>10</v>
-      </c>
-      <c r="E19" s="19"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="4">
-        <f ca="1">SUM(B17:B20)</f>
+        <v>5</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" s="13" customFormat="1">
+      <c r="A20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="11">
+        <v>12</v>
+      </c>
+      <c r="C20" s="11">
+        <v>12</v>
+      </c>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2">
+        <f ca="1">SUM(B18:B21)</f>
         <v>30</v>
       </c>
-      <c r="C20" s="4">
-        <f ca="1">SUM(C17:C20)</f>
+      <c r="C21" s="2">
+        <f ca="1">SUM(C18:C21)</f>
         <v>30</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20">
-        <f ca="1">C20/B20</f>
+      <c r="E21" s="4"/>
+      <c r="F21">
+        <f ca="1">C21/B21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="D21" s="4"/>
-      <c r="E21" s="8"/>
-    </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="11" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="4">
-        <f ca="1">B14+B20</f>
+      <c r="B23" s="2">
+        <f ca="1">B14+B21</f>
         <v>100</v>
       </c>
-      <c r="C22" s="4">
-        <f ca="1">C14+C20</f>
+      <c r="C23" s="2">
+        <f ca="1">C14+C21</f>
         <v>100</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="8"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>

</xml_diff>

<commit_message>
Updated and improved the rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab1/Assignment1Rubric.xlsx
+++ b/Labs/Lab1/Assignment1Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B200E4B1-0BD5-EC4D-8E71-8DCCF9FC458B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3ACFDA-1B79-F544-AC8E-0C625C753D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13640" yWindow="600" windowWidth="12600" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14200" yWindow="660" windowWidth="11920" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
-  <si>
-    <t>CS246 Assignment 1 Rubric</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Possible</t>
   </si>
@@ -78,9 +75,6 @@
     <t>Requirements Doc</t>
   </si>
   <si>
-    <t>Lab 1: Software requirements</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -99,29 +93,41 @@
     <t>Questions ask for requirement details</t>
   </si>
   <si>
-    <t>Questions are relevat to requirements</t>
-  </si>
-  <si>
     <t>Questions cover sufficient scope</t>
   </si>
   <si>
     <t>Constraints, Assumps, Deps</t>
   </si>
   <si>
-    <t>Qs are relevat to requirements</t>
-  </si>
-  <si>
     <t>Qs over sufficient scope</t>
   </si>
   <si>
     <t>As include sufficient detail</t>
+  </si>
+  <si>
+    <t>Contribution Report</t>
+  </si>
+  <si>
+    <t>CS246 Rubric for Assignment 1: Software requirements</t>
+  </si>
+  <si>
+    <t>Qs are relevant to requirements</t>
+  </si>
+  <si>
+    <t>Questions are relevant to requirements</t>
+  </si>
+  <si>
+    <t>Your team did a great job on all aspects of this assignment! It sounds like you also did a good job of collaborating and communicating as a team. I was impressed with the scope and detail of your functional requirements.</t>
+  </si>
+  <si>
+    <t>Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,6 +240,32 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Liberation Serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -330,13 +362,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -362,8 +391,27 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -695,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="129" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -707,165 +755,186 @@
     <col min="2" max="2" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="6"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="8" t="s">
+      <c r="B7" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUM(B4:B7)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
+      <c r="B18">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="8" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2">
+        <f>SUM(B11:B19)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="7"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <f>SUM(B4:B12)</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="9"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUM(B16:B19)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="8"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2">
-        <f>B13+B20</f>
+      <c r="B24" s="2">
+        <f>B20+B8+B22</f>
         <v>100</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
@@ -876,276 +945,306 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" ht="46" customHeight="1">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="6"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="10" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="10">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <f>SUM(B5:B8)</f>
+        <v>30</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUM(C5:C8)</f>
+        <v>30</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9">
+        <f>C9/B9</f>
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="12"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
         <v>2</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2">
+        <f>SUM(B12:B20)</f>
+        <v>62</v>
+      </c>
+      <c r="C21" s="2">
+        <f>SUM(C12:C20)</f>
+        <v>62</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C23" s="2">
         <v>8</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7">
-        <f>C7/B7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <f>SUM(B5:B13)</f>
-        <v>70</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C5:C13)</f>
-        <v>70</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14">
-        <f>C14/B14</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="9"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <v>8</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" s="13" customFormat="1">
-      <c r="A20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="11">
-        <v>12</v>
-      </c>
-      <c r="C20" s="11">
-        <v>12</v>
-      </c>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="2">
-        <f ca="1">SUM(B18:B21)</f>
-        <v>30</v>
-      </c>
-      <c r="C21" s="2">
-        <f ca="1">SUM(C18:C21)</f>
-        <v>30</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21">
-        <f ca="1">C21/B21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="D22" s="2"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="2">
-        <f ca="1">B14+B21</f>
+      <c r="B25" s="2">
+        <f>B21+B9+B23</f>
         <v>100</v>
       </c>
-      <c r="C23" s="2">
-        <f ca="1">C14+C21</f>
+      <c r="C25" s="2">
+        <f>C21+C9+C23</f>
         <v>100</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>

</xml_diff>